<commit_message>
filename change and updates
</commit_message>
<xml_diff>
--- a/crosswalks/SURF_Sample_Types_jr.xlsx
+++ b/crosswalks/SURF_Sample_Types_jr.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michaelw\Documents\R\crosswalks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michaelw\Documents\R\SURFtoCEDEN\crosswalks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Types" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="153">
   <si>
     <t>SAMP_TYPE_CD</t>
   </si>
@@ -472,6 +472,18 @@
   </si>
   <si>
     <t>SampleType Comments</t>
+  </si>
+  <si>
+    <t>SampleType Processing Notes</t>
+  </si>
+  <si>
+    <t>use Not Recorded</t>
+  </si>
+  <si>
+    <t>update MatrixCode &lt;-runoff, if SAMP_TYPE_CD =9</t>
+  </si>
+  <si>
+    <t>update MatrixCode &lt;-runoff, if SAMP_TYPE_CD =10</t>
   </si>
 </sst>
 </file>
@@ -827,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -839,10 +851,11 @@
     <col min="2" max="2" width="84.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="77.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="142.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="47.7109375" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,8 +868,11 @@
       <c r="D1" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -870,7 +886,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -883,8 +899,11 @@
       <c r="D3" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="45.75" x14ac:dyDescent="0.3">
+      <c r="E3" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -898,7 +917,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>6</v>
       </c>
@@ -909,7 +928,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>7</v>
       </c>
@@ -923,7 +942,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>8</v>
       </c>
@@ -937,7 +956,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>9</v>
       </c>
@@ -950,8 +969,11 @@
       <c r="D8" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>10</v>
       </c>
@@ -964,8 +986,11 @@
       <c r="D9" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>11</v>
       </c>
@@ -976,7 +1001,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="45.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>12</v>
       </c>
@@ -990,7 +1015,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>13</v>
       </c>
@@ -1001,7 +1026,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>14</v>
       </c>
@@ -1015,7 +1040,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>15</v>
       </c>

</xml_diff>